<commit_message>
dni client create quote
</commit_message>
<xml_diff>
--- a/target/ExcelCalculatorForDistributor/Arshad New Calculator.xlsx
+++ b/target/ExcelCalculatorForDistributor/Arshad New Calculator.xlsx
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63901" uniqueCount="1316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67271" uniqueCount="1386">
   <si>
     <t>id</t>
   </si>
@@ -4114,6 +4114,216 @@
   </si>
   <si>
     <t>56328</t>
+  </si>
+  <si>
+    <t>56641</t>
+  </si>
+  <si>
+    <t>1729</t>
+  </si>
+  <si>
+    <t>TEST-ABC-0225-1-00010</t>
+  </si>
+  <si>
+    <t>56642</t>
+  </si>
+  <si>
+    <t>56643</t>
+  </si>
+  <si>
+    <t>56644</t>
+  </si>
+  <si>
+    <t>56645</t>
+  </si>
+  <si>
+    <t>56646</t>
+  </si>
+  <si>
+    <t>56647</t>
+  </si>
+  <si>
+    <t>56648</t>
+  </si>
+  <si>
+    <t>56649</t>
+  </si>
+  <si>
+    <t>56650</t>
+  </si>
+  <si>
+    <t>56651</t>
+  </si>
+  <si>
+    <t>56652</t>
+  </si>
+  <si>
+    <t>56653</t>
+  </si>
+  <si>
+    <t>56654</t>
+  </si>
+  <si>
+    <t>56655</t>
+  </si>
+  <si>
+    <t>56656</t>
+  </si>
+  <si>
+    <t>56657</t>
+  </si>
+  <si>
+    <t>56658</t>
+  </si>
+  <si>
+    <t>56659</t>
+  </si>
+  <si>
+    <t>56660</t>
+  </si>
+  <si>
+    <t>56661</t>
+  </si>
+  <si>
+    <t>56662</t>
+  </si>
+  <si>
+    <t>56663</t>
+  </si>
+  <si>
+    <t>56664</t>
+  </si>
+  <si>
+    <t>56665</t>
+  </si>
+  <si>
+    <t>56666</t>
+  </si>
+  <si>
+    <t>56667</t>
+  </si>
+  <si>
+    <t>56668</t>
+  </si>
+  <si>
+    <t>56669</t>
+  </si>
+  <si>
+    <t>56670</t>
+  </si>
+  <si>
+    <t>56671</t>
+  </si>
+  <si>
+    <t>56672</t>
+  </si>
+  <si>
+    <t>56673</t>
+  </si>
+  <si>
+    <t>56674</t>
+  </si>
+  <si>
+    <t>56675</t>
+  </si>
+  <si>
+    <t>56676</t>
+  </si>
+  <si>
+    <t>56677</t>
+  </si>
+  <si>
+    <t>56678</t>
+  </si>
+  <si>
+    <t>56679</t>
+  </si>
+  <si>
+    <t>28635</t>
+  </si>
+  <si>
+    <t>861</t>
+  </si>
+  <si>
+    <t>686.0</t>
+  </si>
+  <si>
+    <t>2025-01-29 12:54:01</t>
+  </si>
+  <si>
+    <t>28636</t>
+  </si>
+  <si>
+    <t>28637</t>
+  </si>
+  <si>
+    <t>28638</t>
+  </si>
+  <si>
+    <t>28639</t>
+  </si>
+  <si>
+    <t>28640</t>
+  </si>
+  <si>
+    <t>ALBANIA</t>
+  </si>
+  <si>
+    <t>10.0</t>
+  </si>
+  <si>
+    <t>Slightly Preferred</t>
+  </si>
+  <si>
+    <t>AFGHANISTAN</t>
+  </si>
+  <si>
+    <t>AMERICAN SAMOA</t>
+  </si>
+  <si>
+    <t>ANTIGUA AND BARBUDA</t>
+  </si>
+  <si>
+    <t>ANGUILLA</t>
+  </si>
+  <si>
+    <t>ANGOLA</t>
+  </si>
+  <si>
+    <t>ARMENIA</t>
+  </si>
+  <si>
+    <t>BAHAMAS</t>
+  </si>
+  <si>
+    <t>ANTARCTICA</t>
+  </si>
+  <si>
+    <t>AZERBAIJAN</t>
+  </si>
+  <si>
+    <t>HUNGARY</t>
+  </si>
+  <si>
+    <t>ALGERIA</t>
+  </si>
+  <si>
+    <t>100.0</t>
+  </si>
+  <si>
+    <t>BURKINA FASO</t>
+  </si>
+  <si>
+    <t>CAPE VERDE</t>
+  </si>
+  <si>
+    <t>CHAD</t>
+  </si>
+  <si>
+    <t>ANDORRA</t>
+  </si>
+  <si>
+    <t>Hospitals, Clinics, Pharmacies and Diagnostic</t>
   </si>
 </sst>
 </file>
@@ -9159,16 +9369,16 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="83" t="s">
-        <v>532</v>
+        <v>1357</v>
       </c>
       <c r="B2" s="83" t="s">
-        <v>533</v>
+        <v>1358</v>
       </c>
       <c r="C2" s="83" t="s">
         <v>308</v>
       </c>
       <c r="D2" s="28" t="s">
-        <v>309</v>
+        <v>332</v>
       </c>
       <c r="E2" s="84" t="s">
         <v>17</v>
@@ -9178,7 +9388,7 @@
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="4" t="s">
-        <v>281</v>
+        <v>1359</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>282</v>
@@ -9189,10 +9399,10 @@
         <v>310</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>534</v>
+        <v>1360</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>534</v>
+        <v>1360</v>
       </c>
       <c r="P2" s="4" t="str">
         <f t="shared" ref="P2:P65" si="0">C2&amp;-D2</f>
@@ -9209,26 +9419,26 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="83" t="s">
-        <v>535</v>
+        <v>1361</v>
       </c>
       <c r="B3" s="83" t="s">
-        <v>533</v>
+        <v>1358</v>
       </c>
       <c r="C3" s="83" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="D3" s="28" t="s">
-        <v>312</v>
+        <v>332</v>
       </c>
       <c r="E3" s="84" t="s">
-        <v>17</v>
+        <v>294</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>18</v>
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="4" t="s">
-        <v>283</v>
+        <v>1359</v>
       </c>
       <c r="I3" s="4" t="s">
         <v>282</v>
@@ -9239,10 +9449,10 @@
         <v>310</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>534</v>
+        <v>1360</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>534</v>
+        <v>1360</v>
       </c>
       <c r="P3" s="4" t="str">
         <f t="shared" si="0"/>
@@ -9259,26 +9469,26 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="83" t="s">
-        <v>536</v>
+        <v>1362</v>
       </c>
       <c r="B4" s="83" t="s">
-        <v>533</v>
+        <v>1358</v>
       </c>
       <c r="C4" s="83" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="D4" s="28" t="s">
-        <v>314</v>
+        <v>332</v>
       </c>
       <c r="E4" s="84" t="s">
-        <v>17</v>
+        <v>304</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>18</v>
       </c>
       <c r="G4" s="4"/>
       <c r="H4" s="4" t="s">
-        <v>284</v>
+        <v>1359</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>282</v>
@@ -9289,10 +9499,10 @@
         <v>310</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>534</v>
+        <v>1360</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>534</v>
+        <v>1360</v>
       </c>
       <c r="P4" s="4" t="str">
         <f t="shared" si="0"/>
@@ -9309,26 +9519,26 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="83" t="s">
-        <v>537</v>
+        <v>1363</v>
       </c>
       <c r="B5" s="83" t="s">
-        <v>533</v>
+        <v>1358</v>
       </c>
       <c r="C5" s="83" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="D5" s="28" t="s">
-        <v>316</v>
+        <v>332</v>
       </c>
       <c r="E5" s="84" t="s">
         <v>17</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>18</v>
+        <v>306</v>
       </c>
       <c r="G5" s="4"/>
       <c r="H5" s="4" t="s">
-        <v>285</v>
+        <v>1359</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>282</v>
@@ -9339,10 +9549,10 @@
         <v>310</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>534</v>
+        <v>1360</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>534</v>
+        <v>1360</v>
       </c>
       <c r="P5" s="4" t="str">
         <f t="shared" si="0"/>
@@ -9359,26 +9569,26 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="83" t="s">
-        <v>538</v>
+        <v>1364</v>
       </c>
       <c r="B6" s="83" t="s">
-        <v>533</v>
+        <v>1358</v>
       </c>
       <c r="C6" s="83" t="s">
-        <v>317</v>
+        <v>308</v>
       </c>
       <c r="D6" s="28" t="s">
-        <v>318</v>
+        <v>332</v>
       </c>
       <c r="E6" s="84" t="s">
-        <v>17</v>
+        <v>294</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>18</v>
+        <v>306</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4" t="s">
-        <v>286</v>
+        <v>1359</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>282</v>
@@ -9389,10 +9599,10 @@
         <v>310</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>534</v>
+        <v>1360</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>534</v>
+        <v>1360</v>
       </c>
       <c r="P6" s="4" t="str">
         <f t="shared" si="0"/>
@@ -9409,26 +9619,26 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="83" t="s">
-        <v>539</v>
+        <v>1365</v>
       </c>
       <c r="B7" s="83" t="s">
-        <v>533</v>
+        <v>1358</v>
       </c>
       <c r="C7" s="83" t="s">
-        <v>319</v>
+        <v>308</v>
       </c>
       <c r="D7" s="28" t="s">
-        <v>320</v>
+        <v>332</v>
       </c>
       <c r="E7" s="84" t="s">
-        <v>17</v>
+        <v>304</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>18</v>
+        <v>306</v>
       </c>
       <c r="G7" s="4"/>
       <c r="H7" s="4" t="s">
-        <v>287</v>
+        <v>1359</v>
       </c>
       <c r="I7" s="4" t="s">
         <v>282</v>
@@ -9439,10 +9649,10 @@
         <v>310</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>534</v>
+        <v>1360</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>534</v>
+        <v>1360</v>
       </c>
       <c r="P7" s="4" t="str">
         <f t="shared" si="0"/>
@@ -44688,7 +44898,7 @@
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" s="163" t="s">
-        <v>1275</v>
+        <v>1316</v>
       </c>
       <c r="B2" s="86" t="s">
         <v>42</v>
@@ -44706,13 +44916,13 @@
         <v>43</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>1276</v>
+        <v>1317</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>1277</v>
+        <v>1318</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>246</v>
@@ -44735,7 +44945,7 @@
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" s="163" t="s">
-        <v>1278</v>
+        <v>1319</v>
       </c>
       <c r="B3" s="86" t="s">
         <v>48</v>
@@ -44753,13 +44963,13 @@
         <v>43</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>1276</v>
+        <v>1317</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>1277</v>
+        <v>1318</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>246</v>
@@ -44782,7 +44992,7 @@
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A4" s="163" t="s">
-        <v>1279</v>
+        <v>1320</v>
       </c>
       <c r="B4" s="86" t="s">
         <v>50</v>
@@ -44800,13 +45010,13 @@
         <v>43</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>1276</v>
+        <v>1317</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>1277</v>
+        <v>1318</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>246</v>
@@ -44829,7 +45039,7 @@
     </row>
     <row r="5" spans="1:25" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="163" t="s">
-        <v>1280</v>
+        <v>1321</v>
       </c>
       <c r="B5" s="86" t="s">
         <v>52</v>
@@ -44847,13 +45057,13 @@
         <v>43</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>1276</v>
+        <v>1317</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>1277</v>
+        <v>1318</v>
       </c>
       <c r="J5" s="3" t="s">
         <v>246</v>
@@ -44876,7 +45086,7 @@
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A6" s="163" t="s">
-        <v>1281</v>
+        <v>1322</v>
       </c>
       <c r="B6" s="86" t="s">
         <v>53</v>
@@ -44894,13 +45104,13 @@
         <v>43</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>1276</v>
+        <v>1317</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>1277</v>
+        <v>1318</v>
       </c>
       <c r="J6" s="3" t="s">
         <v>246</v>
@@ -44923,7 +45133,7 @@
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A7" s="163" t="s">
-        <v>1282</v>
+        <v>1323</v>
       </c>
       <c r="B7" s="86" t="s">
         <v>54</v>
@@ -44941,13 +45151,13 @@
         <v>43</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>1276</v>
+        <v>1317</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>1277</v>
+        <v>1318</v>
       </c>
       <c r="J7" s="3" t="s">
         <v>246</v>
@@ -44970,7 +45180,7 @@
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A8" s="163" t="s">
-        <v>1283</v>
+        <v>1324</v>
       </c>
       <c r="B8" s="86" t="s">
         <v>57</v>
@@ -44988,13 +45198,13 @@
         <v>43</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>1276</v>
+        <v>1317</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>1277</v>
+        <v>1318</v>
       </c>
       <c r="J8" s="3" t="s">
         <v>246</v>
@@ -45017,7 +45227,7 @@
     </row>
     <row r="9" spans="1:25" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="163" t="s">
-        <v>1284</v>
+        <v>1325</v>
       </c>
       <c r="B9" s="86" t="s">
         <v>59</v>
@@ -45035,13 +45245,13 @@
         <v>43</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>1276</v>
+        <v>1317</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>1277</v>
+        <v>1318</v>
       </c>
       <c r="J9" s="3" t="s">
         <v>246</v>
@@ -45064,7 +45274,7 @@
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A10" s="163" t="s">
-        <v>1285</v>
+        <v>1326</v>
       </c>
       <c r="B10" s="86" t="s">
         <v>61</v>
@@ -45082,13 +45292,13 @@
         <v>43</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>1276</v>
+        <v>1317</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>1277</v>
+        <v>1318</v>
       </c>
       <c r="J10" s="3" t="s">
         <v>246</v>
@@ -45111,7 +45321,7 @@
     </row>
     <row r="11" spans="1:25" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" s="163" t="s">
-        <v>1286</v>
+        <v>1327</v>
       </c>
       <c r="B11" s="86" t="s">
         <v>62</v>
@@ -45129,13 +45339,13 @@
         <v>43</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>1276</v>
+        <v>1317</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>1277</v>
+        <v>1318</v>
       </c>
       <c r="J11" s="3" t="s">
         <v>246</v>
@@ -45158,7 +45368,7 @@
     </row>
     <row r="12" spans="1:25" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="163" t="s">
-        <v>1287</v>
+        <v>1328</v>
       </c>
       <c r="B12" s="86" t="s">
         <v>63</v>
@@ -45176,13 +45386,13 @@
         <v>43</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>1276</v>
+        <v>1317</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>1277</v>
+        <v>1318</v>
       </c>
       <c r="J12" s="3" t="s">
         <v>246</v>
@@ -45205,7 +45415,7 @@
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A13" s="163" t="s">
-        <v>1288</v>
+        <v>1329</v>
       </c>
       <c r="B13" s="86" t="s">
         <v>64</v>
@@ -45223,13 +45433,13 @@
         <v>43</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>1276</v>
+        <v>1317</v>
       </c>
       <c r="H13" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>1277</v>
+        <v>1318</v>
       </c>
       <c r="J13" s="3" t="s">
         <v>246</v>
@@ -45252,7 +45462,7 @@
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A14" s="163" t="s">
-        <v>1289</v>
+        <v>1330</v>
       </c>
       <c r="B14" s="86" t="s">
         <v>68</v>
@@ -45270,13 +45480,13 @@
         <v>43</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>1276</v>
+        <v>1317</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>1277</v>
+        <v>1318</v>
       </c>
       <c r="J14" s="3" t="s">
         <v>246</v>
@@ -45299,7 +45509,7 @@
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A15" s="163" t="s">
-        <v>1290</v>
+        <v>1331</v>
       </c>
       <c r="B15" s="86" t="s">
         <v>71</v>
@@ -45317,13 +45527,13 @@
         <v>43</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>1276</v>
+        <v>1317</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>1277</v>
+        <v>1318</v>
       </c>
       <c r="J15" s="3" t="s">
         <v>246</v>
@@ -45346,7 +45556,7 @@
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A16" s="163" t="s">
-        <v>1291</v>
+        <v>1332</v>
       </c>
       <c r="B16" s="86" t="s">
         <v>73</v>
@@ -45364,13 +45574,13 @@
         <v>43</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>1276</v>
+        <v>1317</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>1277</v>
+        <v>1318</v>
       </c>
       <c r="J16" s="3" t="s">
         <v>246</v>
@@ -45393,7 +45603,7 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="163" t="s">
-        <v>1292</v>
+        <v>1333</v>
       </c>
       <c r="B17" s="86" t="s">
         <v>75</v>
@@ -45411,13 +45621,13 @@
         <v>43</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>1276</v>
+        <v>1317</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>1277</v>
+        <v>1318</v>
       </c>
       <c r="J17" s="3" t="s">
         <v>246</v>
@@ -45440,7 +45650,7 @@
     </row>
     <row r="18" spans="1:15" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A18" s="163" t="s">
-        <v>1293</v>
+        <v>1334</v>
       </c>
       <c r="B18" s="86" t="s">
         <v>793</v>
@@ -45458,13 +45668,13 @@
         <v>43</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>1276</v>
+        <v>1317</v>
       </c>
       <c r="H18" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>1277</v>
+        <v>1318</v>
       </c>
       <c r="J18" s="3" t="s">
         <v>246</v>
@@ -45487,7 +45697,7 @@
     </row>
     <row r="19" spans="1:15" ht="72" x14ac:dyDescent="0.3">
       <c r="A19" s="163" t="s">
-        <v>1294</v>
+        <v>1335</v>
       </c>
       <c r="B19" s="86" t="s">
         <v>523</v>
@@ -45505,13 +45715,13 @@
         <v>43</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>1276</v>
+        <v>1317</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>1277</v>
+        <v>1318</v>
       </c>
       <c r="J19" s="3" t="s">
         <v>246</v>
@@ -45534,7 +45744,7 @@
     </row>
     <row r="20" spans="1:15" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A20" s="163" t="s">
-        <v>1295</v>
+        <v>1336</v>
       </c>
       <c r="B20" s="86" t="s">
         <v>524</v>
@@ -45552,13 +45762,13 @@
         <v>43</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>1276</v>
+        <v>1317</v>
       </c>
       <c r="H20" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>1277</v>
+        <v>1318</v>
       </c>
       <c r="J20" s="3" t="s">
         <v>246</v>
@@ -45581,7 +45791,7 @@
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="163" t="s">
-        <v>1296</v>
+        <v>1337</v>
       </c>
       <c r="B21" s="86" t="s">
         <v>82</v>
@@ -45599,13 +45809,13 @@
         <v>43</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>1276</v>
+        <v>1317</v>
       </c>
       <c r="H21" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>1277</v>
+        <v>1318</v>
       </c>
       <c r="J21" s="3" t="s">
         <v>246</v>
@@ -45628,7 +45838,7 @@
     </row>
     <row r="22" spans="1:15" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A22" s="163" t="s">
-        <v>1297</v>
+        <v>1338</v>
       </c>
       <c r="B22" s="86" t="s">
         <v>526</v>
@@ -45646,13 +45856,13 @@
         <v>43</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>1276</v>
+        <v>1317</v>
       </c>
       <c r="H22" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>1277</v>
+        <v>1318</v>
       </c>
       <c r="J22" s="3" t="s">
         <v>246</v>
@@ -45675,7 +45885,7 @@
     </row>
     <row r="23" spans="1:15" ht="144" x14ac:dyDescent="0.3">
       <c r="A23" s="163" t="s">
-        <v>1298</v>
+        <v>1339</v>
       </c>
       <c r="B23" s="86" t="s">
         <v>527</v>
@@ -45693,13 +45903,13 @@
         <v>43</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>1276</v>
+        <v>1317</v>
       </c>
       <c r="H23" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>1277</v>
+        <v>1318</v>
       </c>
       <c r="J23" s="3" t="s">
         <v>246</v>
@@ -45722,7 +45932,7 @@
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" s="163" t="s">
-        <v>1299</v>
+        <v>1340</v>
       </c>
       <c r="B24" s="86" t="s">
         <v>84</v>
@@ -45740,13 +45950,13 @@
         <v>43</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>1276</v>
+        <v>1317</v>
       </c>
       <c r="H24" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>1277</v>
+        <v>1318</v>
       </c>
       <c r="J24" s="3" t="s">
         <v>246</v>
@@ -45769,7 +45979,7 @@
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" s="163" t="s">
-        <v>1300</v>
+        <v>1341</v>
       </c>
       <c r="B25" s="86" t="s">
         <v>85</v>
@@ -45787,13 +45997,13 @@
         <v>43</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>1276</v>
+        <v>1317</v>
       </c>
       <c r="H25" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>1277</v>
+        <v>1318</v>
       </c>
       <c r="J25" s="3" t="s">
         <v>246</v>
@@ -45816,7 +46026,7 @@
     </row>
     <row r="26" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="163" t="s">
-        <v>1301</v>
+        <v>1342</v>
       </c>
       <c r="B26" s="86" t="s">
         <v>88</v>
@@ -45834,13 +46044,13 @@
         <v>43</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>1276</v>
+        <v>1317</v>
       </c>
       <c r="H26" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>1277</v>
+        <v>1318</v>
       </c>
       <c r="J26" s="3" t="s">
         <v>246</v>
@@ -45863,7 +46073,7 @@
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" s="163" t="s">
-        <v>1302</v>
+        <v>1343</v>
       </c>
       <c r="B27" s="86" t="s">
         <v>90</v>
@@ -45881,13 +46091,13 @@
         <v>43</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>1276</v>
+        <v>1317</v>
       </c>
       <c r="H27" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>1277</v>
+        <v>1318</v>
       </c>
       <c r="J27" s="3" t="s">
         <v>246</v>
@@ -45910,7 +46120,7 @@
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" s="163" t="s">
-        <v>1303</v>
+        <v>1344</v>
       </c>
       <c r="B28" s="86" t="s">
         <v>91</v>
@@ -45928,13 +46138,13 @@
         <v>43</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>1276</v>
+        <v>1317</v>
       </c>
       <c r="H28" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>1277</v>
+        <v>1318</v>
       </c>
       <c r="J28" s="3" t="s">
         <v>246</v>
@@ -45957,7 +46167,7 @@
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" s="163" t="s">
-        <v>1304</v>
+        <v>1345</v>
       </c>
       <c r="B29" s="86" t="s">
         <v>95</v>
@@ -45975,13 +46185,13 @@
         <v>43</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>1276</v>
+        <v>1317</v>
       </c>
       <c r="H29" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>1277</v>
+        <v>1318</v>
       </c>
       <c r="J29" s="3" t="s">
         <v>246</v>
@@ -46004,7 +46214,7 @@
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" s="163" t="s">
-        <v>1305</v>
+        <v>1346</v>
       </c>
       <c r="B30" s="86" t="s">
         <v>98</v>
@@ -46022,13 +46232,13 @@
         <v>43</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>1276</v>
+        <v>1317</v>
       </c>
       <c r="H30" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>1277</v>
+        <v>1318</v>
       </c>
       <c r="J30" s="3" t="s">
         <v>246</v>
@@ -46051,7 +46261,7 @@
     </row>
     <row r="31" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="163" t="s">
-        <v>1306</v>
+        <v>1347</v>
       </c>
       <c r="B31" s="86" t="s">
         <v>697</v>
@@ -46069,13 +46279,13 @@
         <v>43</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>1276</v>
+        <v>1317</v>
       </c>
       <c r="H31" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>1277</v>
+        <v>1318</v>
       </c>
       <c r="J31" s="3" t="s">
         <v>246</v>
@@ -46098,7 +46308,7 @@
     </row>
     <row r="32" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="163" t="s">
-        <v>1307</v>
+        <v>1348</v>
       </c>
       <c r="B32" s="86" t="s">
         <v>704</v>
@@ -46116,13 +46326,13 @@
         <v>43</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>1276</v>
+        <v>1317</v>
       </c>
       <c r="H32" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>1277</v>
+        <v>1318</v>
       </c>
       <c r="J32" s="3" t="s">
         <v>246</v>
@@ -46145,7 +46355,7 @@
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33" s="163" t="s">
-        <v>1308</v>
+        <v>1349</v>
       </c>
       <c r="B33" s="86" t="s">
         <v>531</v>
@@ -46163,13 +46373,13 @@
         <v>43</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>1276</v>
+        <v>1317</v>
       </c>
       <c r="H33" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>1277</v>
+        <v>1318</v>
       </c>
       <c r="J33" s="3" t="s">
         <v>246</v>
@@ -46192,7 +46402,7 @@
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34" s="163" t="s">
-        <v>1309</v>
+        <v>1350</v>
       </c>
       <c r="B34" s="86" t="s">
         <v>102</v>
@@ -46210,13 +46420,13 @@
         <v>43</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>1276</v>
+        <v>1317</v>
       </c>
       <c r="H34" s="3" t="s">
         <v>337</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>1277</v>
+        <v>1318</v>
       </c>
       <c r="J34" s="3" t="s">
         <v>246</v>
@@ -46239,7 +46449,7 @@
     </row>
     <row r="35">
       <c r="A35" t="s" s="163">
-        <v>1310</v>
+        <v>1351</v>
       </c>
       <c r="B35" t="s" s="86">
         <v>104</v>
@@ -46257,13 +46467,13 @@
         <v>43</v>
       </c>
       <c r="G35" t="s" s="3">
-        <v>1276</v>
+        <v>1317</v>
       </c>
       <c r="H35" t="s" s="3">
         <v>337</v>
       </c>
       <c r="I35" t="s" s="3">
-        <v>1277</v>
+        <v>1318</v>
       </c>
       <c r="J35" t="s" s="3">
         <v>246</v>
@@ -46286,7 +46496,7 @@
     </row>
     <row r="36">
       <c r="A36" t="s" s="163">
-        <v>1311</v>
+        <v>1352</v>
       </c>
       <c r="B36" t="s" s="86">
         <v>106</v>
@@ -46304,13 +46514,13 @@
         <v>43</v>
       </c>
       <c r="G36" t="s" s="3">
-        <v>1276</v>
+        <v>1317</v>
       </c>
       <c r="H36" t="s" s="3">
         <v>337</v>
       </c>
       <c r="I36" t="s" s="3">
-        <v>1277</v>
+        <v>1318</v>
       </c>
       <c r="J36" t="s" s="3">
         <v>246</v>
@@ -46333,7 +46543,7 @@
     </row>
     <row r="37">
       <c r="A37" t="s" s="163">
-        <v>1312</v>
+        <v>1353</v>
       </c>
       <c r="B37" t="s" s="86">
         <v>722</v>
@@ -46351,13 +46561,13 @@
         <v>43</v>
       </c>
       <c r="G37" t="s" s="3">
-        <v>1276</v>
+        <v>1317</v>
       </c>
       <c r="H37" t="s" s="3">
         <v>337</v>
       </c>
       <c r="I37" t="s" s="3">
-        <v>1277</v>
+        <v>1318</v>
       </c>
       <c r="J37" t="s" s="3">
         <v>246</v>
@@ -46380,7 +46590,7 @@
     </row>
     <row r="38">
       <c r="A38" t="s" s="163">
-        <v>1313</v>
+        <v>1354</v>
       </c>
       <c r="B38" t="s" s="86">
         <v>728</v>
@@ -46398,13 +46608,13 @@
         <v>43</v>
       </c>
       <c r="G38" t="s" s="3">
-        <v>1276</v>
+        <v>1317</v>
       </c>
       <c r="H38" t="s" s="3">
         <v>337</v>
       </c>
       <c r="I38" t="s" s="3">
-        <v>1277</v>
+        <v>1318</v>
       </c>
       <c r="J38" t="s" s="3">
         <v>246</v>
@@ -46427,7 +46637,7 @@
     </row>
     <row r="39">
       <c r="A39" t="s" s="163">
-        <v>1314</v>
+        <v>1355</v>
       </c>
       <c r="B39" t="s" s="86">
         <v>733</v>
@@ -46445,13 +46655,13 @@
         <v>43</v>
       </c>
       <c r="G39" t="s" s="3">
-        <v>1276</v>
+        <v>1317</v>
       </c>
       <c r="H39" t="s" s="3">
         <v>337</v>
       </c>
       <c r="I39" t="s" s="3">
-        <v>1277</v>
+        <v>1318</v>
       </c>
       <c r="J39" t="s" s="3">
         <v>246</v>
@@ -46474,7 +46684,7 @@
     </row>
     <row r="40">
       <c r="A40" t="s" s="163">
-        <v>1315</v>
+        <v>1356</v>
       </c>
       <c r="B40" t="s" s="86">
         <v>738</v>
@@ -46492,13 +46702,13 @@
         <v>43</v>
       </c>
       <c r="G40" t="s" s="3">
-        <v>1276</v>
+        <v>1317</v>
       </c>
       <c r="H40" t="s" s="3">
         <v>337</v>
       </c>
       <c r="I40" t="s" s="3">
-        <v>1277</v>
+        <v>1318</v>
       </c>
       <c r="J40" t="s" s="3">
         <v>246</v>
@@ -55114,7 +55324,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0FDCE05-8D35-4D2B-8CC6-8E3C7553E435}">
-  <dimension ref="A1:P12"/>
+  <dimension ref="A1:P18"/>
   <sheetViews>
     <sheetView zoomScale="109" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -55163,101 +55373,101 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>177</v>
+        <v>187</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>178</v>
+        <v>1366</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>249</v>
+        <v>1367</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>177</v>
+        <v>1368</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>181</v>
+        <v>1369</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>249</v>
+        <v>272</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>177</v>
+        <v>1368</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>183</v>
+        <v>1370</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>249</v>
+        <v>272</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>177</v>
+        <v>187</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>184</v>
+        <v>1371</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>249</v>
+        <v>1367</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>177</v>
+        <v>187</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>185</v>
+        <v>1372</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>249</v>
+        <v>1367</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>177</v>
+        <v>1368</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>186</v>
+        <v>1373</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>249</v>
+        <v>272</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>187</v>
+        <v>1368</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>188</v>
+        <v>1374</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>250</v>
+        <v>272</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>187</v>
+        <v>1368</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>189</v>
+        <v>1375</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>250</v>
+        <v>272</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>191</v>
+        <v>1376</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
@@ -55265,21 +55475,87 @@
         <v>187</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>192</v>
+        <v>1377</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>250</v>
+        <v>1367</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s" s="1">
+        <v>177</v>
+      </c>
+      <c r="B13" t="s" s="1">
+        <v>1378</v>
+      </c>
+      <c r="C13" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s" s="1">
         <v>193</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>251</v>
+      <c r="B14" t="s" s="1">
+        <v>1379</v>
+      </c>
+      <c r="C14" t="s" s="1">
+        <v>1380</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s" s="1">
+        <v>193</v>
+      </c>
+      <c r="B15" t="s" s="1">
+        <v>1381</v>
+      </c>
+      <c r="C15" t="s" s="1">
+        <v>1380</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s" s="1">
+        <v>193</v>
+      </c>
+      <c r="B16" t="s" s="1">
+        <v>1382</v>
+      </c>
+      <c r="C16" t="s" s="1">
+        <v>1380</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s" s="1">
+        <v>193</v>
+      </c>
+      <c r="B17" t="s" s="1">
+        <v>1383</v>
+      </c>
+      <c r="C17" t="s" s="1">
+        <v>1380</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s" s="1">
+        <v>1368</v>
+      </c>
+      <c r="B18" t="s" s="1">
+        <v>1384</v>
+      </c>
+      <c r="C18" t="s" s="1">
+        <v>272</v>
       </c>
     </row>
   </sheetData>
@@ -55294,7 +55570,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{937BFF78-0E8F-43A8-8402-97D478674A28}">
-  <dimension ref="A1:P31"/>
+  <dimension ref="A1:P120"/>
   <sheetViews>
     <sheetView zoomScale="109" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
@@ -55350,7 +55626,7 @@
         <v>252</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>246</v>
+        <v>272</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
@@ -55363,7 +55639,7 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>254</v>
+        <v>1385</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>246</v>
@@ -55371,7 +55647,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>246</v>
@@ -55379,7 +55655,7 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>246</v>
@@ -55387,7 +55663,7 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>246</v>
@@ -55395,7 +55671,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>252</v>
+        <v>257</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>246</v>
@@ -55403,15 +55679,15 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>246</v>
+        <v>272</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>246</v>
@@ -55419,7 +55695,7 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>255</v>
+        <v>1385</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>246</v>
@@ -55427,7 +55703,7 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>246</v>
@@ -55435,7 +55711,7 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>246</v>
@@ -55443,7 +55719,7 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>246</v>
@@ -55451,7 +55727,7 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>246</v>
@@ -55459,15 +55735,15 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>246</v>
+        <v>272</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>246</v>
@@ -55475,7 +55751,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>256</v>
+        <v>1385</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>246</v>
@@ -55483,7 +55759,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>246</v>
@@ -55491,7 +55767,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>246</v>
@@ -55499,7 +55775,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>246</v>
@@ -55507,7 +55783,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>246</v>
@@ -55515,15 +55791,15 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>246</v>
+        <v>272</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>246</v>
@@ -55531,7 +55807,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>257</v>
+        <v>1385</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>246</v>
@@ -55539,7 +55815,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s" s="1">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B26" t="s" s="1">
         <v>246</v>
@@ -55547,7 +55823,7 @@
     </row>
     <row r="27">
       <c r="A27" t="s" s="1">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="B27" t="s" s="1">
         <v>246</v>
@@ -55555,7 +55831,7 @@
     </row>
     <row r="28">
       <c r="A28" t="s" s="1">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="B28" t="s" s="1">
         <v>246</v>
@@ -55563,7 +55839,7 @@
     </row>
     <row r="29">
       <c r="A29" t="s" s="1">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="B29" t="s" s="1">
         <v>246</v>
@@ -55571,17 +55847,729 @@
     </row>
     <row r="30">
       <c r="A30" t="s" s="1">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="B30" t="s" s="1">
-        <v>246</v>
+        <v>272</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="1">
+        <v>253</v>
+      </c>
+      <c r="B31" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s" s="1">
+        <v>1385</v>
+      </c>
+      <c r="B32" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s" s="1">
+        <v>254</v>
+      </c>
+      <c r="B33" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s" s="1">
+        <v>255</v>
+      </c>
+      <c r="B34" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s" s="1">
+        <v>256</v>
+      </c>
+      <c r="B35" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s" s="1">
         <v>257</v>
       </c>
-      <c r="B31" t="s" s="1">
+      <c r="B36" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s" s="1">
+        <v>252</v>
+      </c>
+      <c r="B37" t="s" s="1">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s" s="1">
+        <v>253</v>
+      </c>
+      <c r="B38" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s" s="1">
+        <v>1385</v>
+      </c>
+      <c r="B39" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s" s="1">
+        <v>254</v>
+      </c>
+      <c r="B40" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s" s="1">
+        <v>255</v>
+      </c>
+      <c r="B41" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s" s="1">
+        <v>256</v>
+      </c>
+      <c r="B42" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s" s="1">
+        <v>257</v>
+      </c>
+      <c r="B43" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s" s="1">
+        <v>252</v>
+      </c>
+      <c r="B44" t="s" s="1">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s" s="1">
+        <v>253</v>
+      </c>
+      <c r="B45" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s" s="1">
+        <v>1385</v>
+      </c>
+      <c r="B46" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s" s="1">
+        <v>254</v>
+      </c>
+      <c r="B47" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s" s="1">
+        <v>255</v>
+      </c>
+      <c r="B48" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s" s="1">
+        <v>256</v>
+      </c>
+      <c r="B49" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s" s="1">
+        <v>257</v>
+      </c>
+      <c r="B50" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s" s="1">
+        <v>252</v>
+      </c>
+      <c r="B51" t="s" s="1">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s" s="1">
+        <v>253</v>
+      </c>
+      <c r="B52" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s" s="1">
+        <v>1385</v>
+      </c>
+      <c r="B53" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s" s="1">
+        <v>254</v>
+      </c>
+      <c r="B54" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s" s="1">
+        <v>255</v>
+      </c>
+      <c r="B55" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s" s="1">
+        <v>256</v>
+      </c>
+      <c r="B56" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s" s="1">
+        <v>257</v>
+      </c>
+      <c r="B57" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s" s="1">
+        <v>252</v>
+      </c>
+      <c r="B58" t="s" s="1">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s" s="1">
+        <v>253</v>
+      </c>
+      <c r="B59" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s" s="1">
+        <v>1385</v>
+      </c>
+      <c r="B60" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s" s="1">
+        <v>254</v>
+      </c>
+      <c r="B61" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s" s="1">
+        <v>255</v>
+      </c>
+      <c r="B62" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s" s="1">
+        <v>256</v>
+      </c>
+      <c r="B63" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="s" s="1">
+        <v>257</v>
+      </c>
+      <c r="B64" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s" s="1">
+        <v>252</v>
+      </c>
+      <c r="B65" t="s" s="1">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s" s="1">
+        <v>253</v>
+      </c>
+      <c r="B66" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s" s="1">
+        <v>1385</v>
+      </c>
+      <c r="B67" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="s" s="1">
+        <v>254</v>
+      </c>
+      <c r="B68" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s" s="1">
+        <v>255</v>
+      </c>
+      <c r="B69" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="s" s="1">
+        <v>256</v>
+      </c>
+      <c r="B70" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="s" s="1">
+        <v>257</v>
+      </c>
+      <c r="B71" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="s" s="1">
+        <v>252</v>
+      </c>
+      <c r="B72" t="s" s="1">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="s" s="1">
+        <v>253</v>
+      </c>
+      <c r="B73" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="s" s="1">
+        <v>1385</v>
+      </c>
+      <c r="B74" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="s" s="1">
+        <v>254</v>
+      </c>
+      <c r="B75" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="s" s="1">
+        <v>255</v>
+      </c>
+      <c r="B76" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="s" s="1">
+        <v>256</v>
+      </c>
+      <c r="B77" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="s" s="1">
+        <v>257</v>
+      </c>
+      <c r="B78" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="s" s="1">
+        <v>252</v>
+      </c>
+      <c r="B79" t="s" s="1">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="s" s="1">
+        <v>253</v>
+      </c>
+      <c r="B80" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="s" s="1">
+        <v>1385</v>
+      </c>
+      <c r="B81" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="s" s="1">
+        <v>254</v>
+      </c>
+      <c r="B82" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="s" s="1">
+        <v>255</v>
+      </c>
+      <c r="B83" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="s" s="1">
+        <v>256</v>
+      </c>
+      <c r="B84" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="s" s="1">
+        <v>257</v>
+      </c>
+      <c r="B85" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="s" s="1">
+        <v>252</v>
+      </c>
+      <c r="B86" t="s" s="1">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="s" s="1">
+        <v>253</v>
+      </c>
+      <c r="B87" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="s" s="1">
+        <v>1385</v>
+      </c>
+      <c r="B88" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="s" s="1">
+        <v>254</v>
+      </c>
+      <c r="B89" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="s" s="1">
+        <v>255</v>
+      </c>
+      <c r="B90" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="s" s="1">
+        <v>256</v>
+      </c>
+      <c r="B91" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="s" s="1">
+        <v>257</v>
+      </c>
+      <c r="B92" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="s" s="1">
+        <v>252</v>
+      </c>
+      <c r="B93" t="s" s="1">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="s" s="1">
+        <v>253</v>
+      </c>
+      <c r="B94" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="s" s="1">
+        <v>1385</v>
+      </c>
+      <c r="B95" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="s" s="1">
+        <v>254</v>
+      </c>
+      <c r="B96" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="s" s="1">
+        <v>255</v>
+      </c>
+      <c r="B97" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="s" s="1">
+        <v>256</v>
+      </c>
+      <c r="B98" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="s" s="1">
+        <v>257</v>
+      </c>
+      <c r="B99" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="s" s="1">
+        <v>252</v>
+      </c>
+      <c r="B100" t="s" s="1">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="s" s="1">
+        <v>253</v>
+      </c>
+      <c r="B101" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="s" s="1">
+        <v>1385</v>
+      </c>
+      <c r="B102" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="s" s="1">
+        <v>254</v>
+      </c>
+      <c r="B103" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="s" s="1">
+        <v>255</v>
+      </c>
+      <c r="B104" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="s" s="1">
+        <v>256</v>
+      </c>
+      <c r="B105" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="s" s="1">
+        <v>257</v>
+      </c>
+      <c r="B106" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="s" s="1">
+        <v>252</v>
+      </c>
+      <c r="B107" t="s" s="1">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="s" s="1">
+        <v>253</v>
+      </c>
+      <c r="B108" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="s" s="1">
+        <v>1385</v>
+      </c>
+      <c r="B109" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="s" s="1">
+        <v>254</v>
+      </c>
+      <c r="B110" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="s" s="1">
+        <v>255</v>
+      </c>
+      <c r="B111" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="s" s="1">
+        <v>256</v>
+      </c>
+      <c r="B112" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="s" s="1">
+        <v>257</v>
+      </c>
+      <c r="B113" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="s" s="1">
+        <v>252</v>
+      </c>
+      <c r="B114" t="s" s="1">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="s" s="1">
+        <v>253</v>
+      </c>
+      <c r="B115" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="s" s="1">
+        <v>1385</v>
+      </c>
+      <c r="B116" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="s" s="1">
+        <v>254</v>
+      </c>
+      <c r="B117" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="s" s="1">
+        <v>255</v>
+      </c>
+      <c r="B118" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="s" s="1">
+        <v>256</v>
+      </c>
+      <c r="B119" t="s" s="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="s" s="1">
+        <v>257</v>
+      </c>
+      <c r="B120" t="s" s="1">
         <v>246</v>
       </c>
     </row>
@@ -55595,7 +56583,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94A9421B-ED15-4F79-A02C-835BE7F65A62}">
-  <dimension ref="A1:P51"/>
+  <dimension ref="A1:P171"/>
   <sheetViews>
     <sheetView zoomScale="109" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -55650,7 +56638,7 @@
         <v>258</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>246</v>
+        <v>259</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
@@ -55661,7 +56649,7 @@
         <v>260</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>246</v>
+        <v>261</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
@@ -55672,7 +56660,7 @@
         <v>262</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>246</v>
+        <v>261</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
@@ -55683,7 +56671,7 @@
         <v>263</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>246</v>
+        <v>261</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
@@ -55694,7 +56682,7 @@
         <v>264</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>246</v>
+        <v>261</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
@@ -55705,7 +56693,7 @@
         <v>265</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>246</v>
+        <v>261</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
@@ -55716,7 +56704,7 @@
         <v>266</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>246</v>
+        <v>261</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
@@ -55727,7 +56715,7 @@
         <v>267</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>246</v>
+        <v>268</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
@@ -55738,7 +56726,7 @@
         <v>269</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>246</v>
+        <v>268</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
@@ -55749,7 +56737,7 @@
         <v>270</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>246</v>
+        <v>268</v>
       </c>
     </row>
     <row r="12">
@@ -55760,7 +56748,7 @@
         <v>258</v>
       </c>
       <c r="C12" t="s" s="1">
-        <v>246</v>
+        <v>259</v>
       </c>
     </row>
     <row r="13">
@@ -55771,7 +56759,7 @@
         <v>260</v>
       </c>
       <c r="C13" t="s" s="1">
-        <v>246</v>
+        <v>261</v>
       </c>
     </row>
     <row r="14">
@@ -55782,7 +56770,7 @@
         <v>262</v>
       </c>
       <c r="C14" t="s" s="1">
-        <v>246</v>
+        <v>261</v>
       </c>
     </row>
     <row r="15">
@@ -55793,7 +56781,7 @@
         <v>263</v>
       </c>
       <c r="C15" t="s" s="1">
-        <v>246</v>
+        <v>261</v>
       </c>
     </row>
     <row r="16">
@@ -55804,7 +56792,7 @@
         <v>264</v>
       </c>
       <c r="C16" t="s" s="1">
-        <v>246</v>
+        <v>261</v>
       </c>
     </row>
     <row r="17">
@@ -55815,7 +56803,7 @@
         <v>265</v>
       </c>
       <c r="C17" t="s" s="1">
-        <v>246</v>
+        <v>261</v>
       </c>
     </row>
     <row r="18">
@@ -55826,7 +56814,7 @@
         <v>266</v>
       </c>
       <c r="C18" t="s" s="1">
-        <v>246</v>
+        <v>261</v>
       </c>
     </row>
     <row r="19">
@@ -55837,7 +56825,7 @@
         <v>267</v>
       </c>
       <c r="C19" t="s" s="1">
-        <v>246</v>
+        <v>268</v>
       </c>
     </row>
     <row r="20">
@@ -55848,7 +56836,7 @@
         <v>269</v>
       </c>
       <c r="C20" t="s" s="1">
-        <v>246</v>
+        <v>268</v>
       </c>
     </row>
     <row r="21">
@@ -55859,7 +56847,7 @@
         <v>270</v>
       </c>
       <c r="C21" t="s" s="1">
-        <v>246</v>
+        <v>268</v>
       </c>
     </row>
     <row r="22">
@@ -55870,7 +56858,7 @@
         <v>258</v>
       </c>
       <c r="C22" t="s" s="1">
-        <v>246</v>
+        <v>259</v>
       </c>
     </row>
     <row r="23">
@@ -55881,7 +56869,7 @@
         <v>260</v>
       </c>
       <c r="C23" t="s" s="1">
-        <v>246</v>
+        <v>261</v>
       </c>
     </row>
     <row r="24">
@@ -55892,7 +56880,7 @@
         <v>262</v>
       </c>
       <c r="C24" t="s" s="1">
-        <v>246</v>
+        <v>261</v>
       </c>
     </row>
     <row r="25">
@@ -55903,7 +56891,7 @@
         <v>263</v>
       </c>
       <c r="C25" t="s" s="1">
-        <v>246</v>
+        <v>261</v>
       </c>
     </row>
     <row r="26">
@@ -55914,7 +56902,7 @@
         <v>264</v>
       </c>
       <c r="C26" t="s" s="1">
-        <v>246</v>
+        <v>261</v>
       </c>
     </row>
     <row r="27">
@@ -55925,7 +56913,7 @@
         <v>265</v>
       </c>
       <c r="C27" t="s" s="1">
-        <v>246</v>
+        <v>261</v>
       </c>
     </row>
     <row r="28">
@@ -55936,7 +56924,7 @@
         <v>266</v>
       </c>
       <c r="C28" t="s" s="1">
-        <v>246</v>
+        <v>261</v>
       </c>
     </row>
     <row r="29">
@@ -55947,7 +56935,7 @@
         <v>267</v>
       </c>
       <c r="C29" t="s" s="1">
-        <v>246</v>
+        <v>268</v>
       </c>
     </row>
     <row r="30">
@@ -55958,7 +56946,7 @@
         <v>269</v>
       </c>
       <c r="C30" t="s" s="1">
-        <v>246</v>
+        <v>268</v>
       </c>
     </row>
     <row r="31">
@@ -55969,7 +56957,7 @@
         <v>270</v>
       </c>
       <c r="C31" t="s" s="1">
-        <v>246</v>
+        <v>268</v>
       </c>
     </row>
     <row r="32">
@@ -55980,7 +56968,7 @@
         <v>258</v>
       </c>
       <c r="C32" t="s" s="1">
-        <v>246</v>
+        <v>259</v>
       </c>
     </row>
     <row r="33">
@@ -55991,7 +56979,7 @@
         <v>260</v>
       </c>
       <c r="C33" t="s" s="1">
-        <v>246</v>
+        <v>261</v>
       </c>
     </row>
     <row r="34">
@@ -56002,7 +56990,7 @@
         <v>262</v>
       </c>
       <c r="C34" t="s" s="1">
-        <v>246</v>
+        <v>261</v>
       </c>
     </row>
     <row r="35">
@@ -56013,7 +57001,7 @@
         <v>263</v>
       </c>
       <c r="C35" t="s" s="1">
-        <v>246</v>
+        <v>261</v>
       </c>
     </row>
     <row r="36">
@@ -56024,7 +57012,7 @@
         <v>264</v>
       </c>
       <c r="C36" t="s" s="1">
-        <v>246</v>
+        <v>261</v>
       </c>
     </row>
     <row r="37">
@@ -56035,7 +57023,7 @@
         <v>265</v>
       </c>
       <c r="C37" t="s" s="1">
-        <v>246</v>
+        <v>261</v>
       </c>
     </row>
     <row r="38">
@@ -56046,7 +57034,7 @@
         <v>266</v>
       </c>
       <c r="C38" t="s" s="1">
-        <v>246</v>
+        <v>261</v>
       </c>
     </row>
     <row r="39">
@@ -56057,7 +57045,7 @@
         <v>267</v>
       </c>
       <c r="C39" t="s" s="1">
-        <v>246</v>
+        <v>268</v>
       </c>
     </row>
     <row r="40">
@@ -56068,7 +57056,7 @@
         <v>269</v>
       </c>
       <c r="C40" t="s" s="1">
-        <v>246</v>
+        <v>268</v>
       </c>
     </row>
     <row r="41">
@@ -56079,7 +57067,7 @@
         <v>270</v>
       </c>
       <c r="C41" t="s" s="1">
-        <v>246</v>
+        <v>268</v>
       </c>
     </row>
     <row r="42">
@@ -56090,7 +57078,7 @@
         <v>258</v>
       </c>
       <c r="C42" t="s" s="1">
-        <v>246</v>
+        <v>259</v>
       </c>
     </row>
     <row r="43">
@@ -56101,7 +57089,7 @@
         <v>260</v>
       </c>
       <c r="C43" t="s" s="1">
-        <v>246</v>
+        <v>261</v>
       </c>
     </row>
     <row r="44">
@@ -56112,7 +57100,7 @@
         <v>262</v>
       </c>
       <c r="C44" t="s" s="1">
-        <v>246</v>
+        <v>261</v>
       </c>
     </row>
     <row r="45">
@@ -56123,7 +57111,7 @@
         <v>263</v>
       </c>
       <c r="C45" t="s" s="1">
-        <v>246</v>
+        <v>261</v>
       </c>
     </row>
     <row r="46">
@@ -56134,7 +57122,7 @@
         <v>264</v>
       </c>
       <c r="C46" t="s" s="1">
-        <v>246</v>
+        <v>261</v>
       </c>
     </row>
     <row r="47">
@@ -56145,7 +57133,7 @@
         <v>265</v>
       </c>
       <c r="C47" t="s" s="1">
-        <v>246</v>
+        <v>261</v>
       </c>
     </row>
     <row r="48">
@@ -56156,7 +57144,7 @@
         <v>266</v>
       </c>
       <c r="C48" t="s" s="1">
-        <v>246</v>
+        <v>261</v>
       </c>
     </row>
     <row r="49">
@@ -56167,7 +57155,7 @@
         <v>267</v>
       </c>
       <c r="C49" t="s" s="1">
-        <v>246</v>
+        <v>268</v>
       </c>
     </row>
     <row r="50">
@@ -56178,7 +57166,7 @@
         <v>269</v>
       </c>
       <c r="C50" t="s" s="1">
-        <v>246</v>
+        <v>268</v>
       </c>
     </row>
     <row r="51">
@@ -56189,7 +57177,1327 @@
         <v>270</v>
       </c>
       <c r="C51" t="s" s="1">
-        <v>246</v>
+        <v>268</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s" s="1">
+        <v>179</v>
+      </c>
+      <c r="B52" t="s" s="1">
+        <v>258</v>
+      </c>
+      <c r="C52" t="s" s="1">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B53" t="s" s="1">
+        <v>260</v>
+      </c>
+      <c r="C53" t="s" s="1">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B54" t="s" s="1">
+        <v>262</v>
+      </c>
+      <c r="C54" t="s" s="1">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B55" t="s" s="1">
+        <v>263</v>
+      </c>
+      <c r="C55" t="s" s="1">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B56" t="s" s="1">
+        <v>264</v>
+      </c>
+      <c r="C56" t="s" s="1">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B57" t="s" s="1">
+        <v>265</v>
+      </c>
+      <c r="C57" t="s" s="1">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B58" t="s" s="1">
+        <v>266</v>
+      </c>
+      <c r="C58" t="s" s="1">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s" s="1">
+        <v>190</v>
+      </c>
+      <c r="B59" t="s" s="1">
+        <v>267</v>
+      </c>
+      <c r="C59" t="s" s="1">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s" s="1">
+        <v>190</v>
+      </c>
+      <c r="B60" t="s" s="1">
+        <v>269</v>
+      </c>
+      <c r="C60" t="s" s="1">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s" s="1">
+        <v>190</v>
+      </c>
+      <c r="B61" t="s" s="1">
+        <v>270</v>
+      </c>
+      <c r="C61" t="s" s="1">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s" s="1">
+        <v>179</v>
+      </c>
+      <c r="B62" t="s" s="1">
+        <v>258</v>
+      </c>
+      <c r="C62" t="s" s="1">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B63" t="s" s="1">
+        <v>260</v>
+      </c>
+      <c r="C63" t="s" s="1">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B64" t="s" s="1">
+        <v>262</v>
+      </c>
+      <c r="C64" t="s" s="1">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B65" t="s" s="1">
+        <v>263</v>
+      </c>
+      <c r="C65" t="s" s="1">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B66" t="s" s="1">
+        <v>264</v>
+      </c>
+      <c r="C66" t="s" s="1">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B67" t="s" s="1">
+        <v>265</v>
+      </c>
+      <c r="C67" t="s" s="1">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B68" t="s" s="1">
+        <v>266</v>
+      </c>
+      <c r="C68" t="s" s="1">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s" s="1">
+        <v>190</v>
+      </c>
+      <c r="B69" t="s" s="1">
+        <v>267</v>
+      </c>
+      <c r="C69" t="s" s="1">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="s" s="1">
+        <v>190</v>
+      </c>
+      <c r="B70" t="s" s="1">
+        <v>269</v>
+      </c>
+      <c r="C70" t="s" s="1">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="s" s="1">
+        <v>190</v>
+      </c>
+      <c r="B71" t="s" s="1">
+        <v>270</v>
+      </c>
+      <c r="C71" t="s" s="1">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="s" s="1">
+        <v>179</v>
+      </c>
+      <c r="B72" t="s" s="1">
+        <v>258</v>
+      </c>
+      <c r="C72" t="s" s="1">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B73" t="s" s="1">
+        <v>260</v>
+      </c>
+      <c r="C73" t="s" s="1">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B74" t="s" s="1">
+        <v>262</v>
+      </c>
+      <c r="C74" t="s" s="1">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B75" t="s" s="1">
+        <v>263</v>
+      </c>
+      <c r="C75" t="s" s="1">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B76" t="s" s="1">
+        <v>264</v>
+      </c>
+      <c r="C76" t="s" s="1">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B77" t="s" s="1">
+        <v>265</v>
+      </c>
+      <c r="C77" t="s" s="1">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B78" t="s" s="1">
+        <v>266</v>
+      </c>
+      <c r="C78" t="s" s="1">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="s" s="1">
+        <v>190</v>
+      </c>
+      <c r="B79" t="s" s="1">
+        <v>267</v>
+      </c>
+      <c r="C79" t="s" s="1">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="s" s="1">
+        <v>190</v>
+      </c>
+      <c r="B80" t="s" s="1">
+        <v>269</v>
+      </c>
+      <c r="C80" t="s" s="1">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="s" s="1">
+        <v>190</v>
+      </c>
+      <c r="B81" t="s" s="1">
+        <v>270</v>
+      </c>
+      <c r="C81" t="s" s="1">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="s" s="1">
+        <v>179</v>
+      </c>
+      <c r="B82" t="s" s="1">
+        <v>258</v>
+      </c>
+      <c r="C82" t="s" s="1">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B83" t="s" s="1">
+        <v>260</v>
+      </c>
+      <c r="C83" t="s" s="1">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B84" t="s" s="1">
+        <v>262</v>
+      </c>
+      <c r="C84" t="s" s="1">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B85" t="s" s="1">
+        <v>263</v>
+      </c>
+      <c r="C85" t="s" s="1">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B86" t="s" s="1">
+        <v>264</v>
+      </c>
+      <c r="C86" t="s" s="1">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B87" t="s" s="1">
+        <v>265</v>
+      </c>
+      <c r="C87" t="s" s="1">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B88" t="s" s="1">
+        <v>266</v>
+      </c>
+      <c r="C88" t="s" s="1">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="s" s="1">
+        <v>190</v>
+      </c>
+      <c r="B89" t="s" s="1">
+        <v>267</v>
+      </c>
+      <c r="C89" t="s" s="1">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="s" s="1">
+        <v>190</v>
+      </c>
+      <c r="B90" t="s" s="1">
+        <v>269</v>
+      </c>
+      <c r="C90" t="s" s="1">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="s" s="1">
+        <v>190</v>
+      </c>
+      <c r="B91" t="s" s="1">
+        <v>270</v>
+      </c>
+      <c r="C91" t="s" s="1">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="s" s="1">
+        <v>179</v>
+      </c>
+      <c r="B92" t="s" s="1">
+        <v>258</v>
+      </c>
+      <c r="C92" t="s" s="1">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B93" t="s" s="1">
+        <v>260</v>
+      </c>
+      <c r="C93" t="s" s="1">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B94" t="s" s="1">
+        <v>262</v>
+      </c>
+      <c r="C94" t="s" s="1">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B95" t="s" s="1">
+        <v>263</v>
+      </c>
+      <c r="C95" t="s" s="1">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B96" t="s" s="1">
+        <v>264</v>
+      </c>
+      <c r="C96" t="s" s="1">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B97" t="s" s="1">
+        <v>265</v>
+      </c>
+      <c r="C97" t="s" s="1">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B98" t="s" s="1">
+        <v>266</v>
+      </c>
+      <c r="C98" t="s" s="1">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="s" s="1">
+        <v>190</v>
+      </c>
+      <c r="B99" t="s" s="1">
+        <v>267</v>
+      </c>
+      <c r="C99" t="s" s="1">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="s" s="1">
+        <v>190</v>
+      </c>
+      <c r="B100" t="s" s="1">
+        <v>269</v>
+      </c>
+      <c r="C100" t="s" s="1">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="s" s="1">
+        <v>190</v>
+      </c>
+      <c r="B101" t="s" s="1">
+        <v>270</v>
+      </c>
+      <c r="C101" t="s" s="1">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="s" s="1">
+        <v>179</v>
+      </c>
+      <c r="B102" t="s" s="1">
+        <v>258</v>
+      </c>
+      <c r="C102" t="s" s="1">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B103" t="s" s="1">
+        <v>260</v>
+      </c>
+      <c r="C103" t="s" s="1">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B104" t="s" s="1">
+        <v>262</v>
+      </c>
+      <c r="C104" t="s" s="1">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B105" t="s" s="1">
+        <v>263</v>
+      </c>
+      <c r="C105" t="s" s="1">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B106" t="s" s="1">
+        <v>264</v>
+      </c>
+      <c r="C106" t="s" s="1">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B107" t="s" s="1">
+        <v>265</v>
+      </c>
+      <c r="C107" t="s" s="1">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B108" t="s" s="1">
+        <v>266</v>
+      </c>
+      <c r="C108" t="s" s="1">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="s" s="1">
+        <v>190</v>
+      </c>
+      <c r="B109" t="s" s="1">
+        <v>267</v>
+      </c>
+      <c r="C109" t="s" s="1">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="s" s="1">
+        <v>190</v>
+      </c>
+      <c r="B110" t="s" s="1">
+        <v>269</v>
+      </c>
+      <c r="C110" t="s" s="1">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="s" s="1">
+        <v>190</v>
+      </c>
+      <c r="B111" t="s" s="1">
+        <v>270</v>
+      </c>
+      <c r="C111" t="s" s="1">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="s" s="1">
+        <v>179</v>
+      </c>
+      <c r="B112" t="s" s="1">
+        <v>258</v>
+      </c>
+      <c r="C112" t="s" s="1">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B113" t="s" s="1">
+        <v>260</v>
+      </c>
+      <c r="C113" t="s" s="1">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B114" t="s" s="1">
+        <v>262</v>
+      </c>
+      <c r="C114" t="s" s="1">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B115" t="s" s="1">
+        <v>263</v>
+      </c>
+      <c r="C115" t="s" s="1">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B116" t="s" s="1">
+        <v>264</v>
+      </c>
+      <c r="C116" t="s" s="1">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B117" t="s" s="1">
+        <v>265</v>
+      </c>
+      <c r="C117" t="s" s="1">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B118" t="s" s="1">
+        <v>266</v>
+      </c>
+      <c r="C118" t="s" s="1">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="s" s="1">
+        <v>190</v>
+      </c>
+      <c r="B119" t="s" s="1">
+        <v>267</v>
+      </c>
+      <c r="C119" t="s" s="1">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="s" s="1">
+        <v>190</v>
+      </c>
+      <c r="B120" t="s" s="1">
+        <v>269</v>
+      </c>
+      <c r="C120" t="s" s="1">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="s" s="1">
+        <v>190</v>
+      </c>
+      <c r="B121" t="s" s="1">
+        <v>270</v>
+      </c>
+      <c r="C121" t="s" s="1">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="s" s="1">
+        <v>179</v>
+      </c>
+      <c r="B122" t="s" s="1">
+        <v>258</v>
+      </c>
+      <c r="C122" t="s" s="1">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B123" t="s" s="1">
+        <v>260</v>
+      </c>
+      <c r="C123" t="s" s="1">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B124" t="s" s="1">
+        <v>262</v>
+      </c>
+      <c r="C124" t="s" s="1">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B125" t="s" s="1">
+        <v>263</v>
+      </c>
+      <c r="C125" t="s" s="1">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B126" t="s" s="1">
+        <v>264</v>
+      </c>
+      <c r="C126" t="s" s="1">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B127" t="s" s="1">
+        <v>265</v>
+      </c>
+      <c r="C127" t="s" s="1">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B128" t="s" s="1">
+        <v>266</v>
+      </c>
+      <c r="C128" t="s" s="1">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="s" s="1">
+        <v>190</v>
+      </c>
+      <c r="B129" t="s" s="1">
+        <v>267</v>
+      </c>
+      <c r="C129" t="s" s="1">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="s" s="1">
+        <v>190</v>
+      </c>
+      <c r="B130" t="s" s="1">
+        <v>269</v>
+      </c>
+      <c r="C130" t="s" s="1">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="s" s="1">
+        <v>190</v>
+      </c>
+      <c r="B131" t="s" s="1">
+        <v>270</v>
+      </c>
+      <c r="C131" t="s" s="1">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="s" s="1">
+        <v>179</v>
+      </c>
+      <c r="B132" t="s" s="1">
+        <v>258</v>
+      </c>
+      <c r="C132" t="s" s="1">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B133" t="s" s="1">
+        <v>260</v>
+      </c>
+      <c r="C133" t="s" s="1">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B134" t="s" s="1">
+        <v>262</v>
+      </c>
+      <c r="C134" t="s" s="1">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B135" t="s" s="1">
+        <v>263</v>
+      </c>
+      <c r="C135" t="s" s="1">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B136" t="s" s="1">
+        <v>264</v>
+      </c>
+      <c r="C136" t="s" s="1">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B137" t="s" s="1">
+        <v>265</v>
+      </c>
+      <c r="C137" t="s" s="1">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B138" t="s" s="1">
+        <v>266</v>
+      </c>
+      <c r="C138" t="s" s="1">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="s" s="1">
+        <v>190</v>
+      </c>
+      <c r="B139" t="s" s="1">
+        <v>267</v>
+      </c>
+      <c r="C139" t="s" s="1">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="s" s="1">
+        <v>190</v>
+      </c>
+      <c r="B140" t="s" s="1">
+        <v>269</v>
+      </c>
+      <c r="C140" t="s" s="1">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="s" s="1">
+        <v>190</v>
+      </c>
+      <c r="B141" t="s" s="1">
+        <v>270</v>
+      </c>
+      <c r="C141" t="s" s="1">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="s" s="1">
+        <v>179</v>
+      </c>
+      <c r="B142" t="s" s="1">
+        <v>258</v>
+      </c>
+      <c r="C142" t="s" s="1">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B143" t="s" s="1">
+        <v>260</v>
+      </c>
+      <c r="C143" t="s" s="1">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B144" t="s" s="1">
+        <v>262</v>
+      </c>
+      <c r="C144" t="s" s="1">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B145" t="s" s="1">
+        <v>263</v>
+      </c>
+      <c r="C145" t="s" s="1">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B146" t="s" s="1">
+        <v>264</v>
+      </c>
+      <c r="C146" t="s" s="1">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B147" t="s" s="1">
+        <v>265</v>
+      </c>
+      <c r="C147" t="s" s="1">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B148" t="s" s="1">
+        <v>266</v>
+      </c>
+      <c r="C148" t="s" s="1">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="s" s="1">
+        <v>190</v>
+      </c>
+      <c r="B149" t="s" s="1">
+        <v>267</v>
+      </c>
+      <c r="C149" t="s" s="1">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="s" s="1">
+        <v>190</v>
+      </c>
+      <c r="B150" t="s" s="1">
+        <v>269</v>
+      </c>
+      <c r="C150" t="s" s="1">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="s" s="1">
+        <v>190</v>
+      </c>
+      <c r="B151" t="s" s="1">
+        <v>270</v>
+      </c>
+      <c r="C151" t="s" s="1">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="s" s="1">
+        <v>179</v>
+      </c>
+      <c r="B152" t="s" s="1">
+        <v>258</v>
+      </c>
+      <c r="C152" t="s" s="1">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B153" t="s" s="1">
+        <v>260</v>
+      </c>
+      <c r="C153" t="s" s="1">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B154" t="s" s="1">
+        <v>262</v>
+      </c>
+      <c r="C154" t="s" s="1">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B155" t="s" s="1">
+        <v>263</v>
+      </c>
+      <c r="C155" t="s" s="1">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B156" t="s" s="1">
+        <v>264</v>
+      </c>
+      <c r="C156" t="s" s="1">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B157" t="s" s="1">
+        <v>265</v>
+      </c>
+      <c r="C157" t="s" s="1">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B158" t="s" s="1">
+        <v>266</v>
+      </c>
+      <c r="C158" t="s" s="1">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="s" s="1">
+        <v>190</v>
+      </c>
+      <c r="B159" t="s" s="1">
+        <v>267</v>
+      </c>
+      <c r="C159" t="s" s="1">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="s" s="1">
+        <v>190</v>
+      </c>
+      <c r="B160" t="s" s="1">
+        <v>269</v>
+      </c>
+      <c r="C160" t="s" s="1">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="s" s="1">
+        <v>190</v>
+      </c>
+      <c r="B161" t="s" s="1">
+        <v>270</v>
+      </c>
+      <c r="C161" t="s" s="1">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="s" s="1">
+        <v>179</v>
+      </c>
+      <c r="B162" t="s" s="1">
+        <v>258</v>
+      </c>
+      <c r="C162" t="s" s="1">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B163" t="s" s="1">
+        <v>260</v>
+      </c>
+      <c r="C163" t="s" s="1">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B164" t="s" s="1">
+        <v>262</v>
+      </c>
+      <c r="C164" t="s" s="1">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B165" t="s" s="1">
+        <v>263</v>
+      </c>
+      <c r="C165" t="s" s="1">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B166" t="s" s="1">
+        <v>264</v>
+      </c>
+      <c r="C166" t="s" s="1">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B167" t="s" s="1">
+        <v>265</v>
+      </c>
+      <c r="C167" t="s" s="1">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="s" s="1">
+        <v>182</v>
+      </c>
+      <c r="B168" t="s" s="1">
+        <v>266</v>
+      </c>
+      <c r="C168" t="s" s="1">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="s" s="1">
+        <v>190</v>
+      </c>
+      <c r="B169" t="s" s="1">
+        <v>267</v>
+      </c>
+      <c r="C169" t="s" s="1">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="s" s="1">
+        <v>190</v>
+      </c>
+      <c r="B170" t="s" s="1">
+        <v>269</v>
+      </c>
+      <c r="C170" t="s" s="1">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="s" s="1">
+        <v>190</v>
+      </c>
+      <c r="B171" t="s" s="1">
+        <v>270</v>
+      </c>
+      <c r="C171" t="s" s="1">
+        <v>268</v>
       </c>
     </row>
   </sheetData>

</xml_diff>